<commit_message>
funciona, falta organizar rutas
</commit_message>
<xml_diff>
--- a/registros_excel/2024-01-25.xlsx
+++ b/registros_excel/2024-01-25.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,10 +453,15 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Area</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Fecha</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Hora</t>
         </is>
@@ -465,22 +470,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1054398414</t>
+          <t>2323232323</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Julian Largo</t>
+          <t>Fabio Castada</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Comercial</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>2024-01-25</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>13:15:26</t>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>22:4:13</t>
         </is>
       </c>
     </row>
@@ -497,12 +507,17 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>2024-01-25</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>13:17:14</t>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>22:5:54</t>
         </is>
       </c>
     </row>
@@ -519,34 +534,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Administrativa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>2024-01-25</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>14:15:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>15961357</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Mauricio Sanchez</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2024-01-25</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>16:57:40</t>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>22:7:54</t>
         </is>
       </c>
     </row>

</xml_diff>